<commit_message>
with 'ready for breakout'
</commit_message>
<xml_diff>
--- a/Gaming/Stocks/Pattern_Statistics/constraints.xlsx
+++ b/Gaming/Stocks/Pattern_Statistics/constraints.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Constraints_2018-07-23" sheetId="1" r:id="rId1"/>
+    <sheet name="Constraints_2018-07-31" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
   <si>
     <t>Constraint</t>
   </si>
@@ -28,7 +28,7 @@
     <t>f_lower_percentage_bounds</t>
   </si>
   <si>
-    <t>f_upper_lower_relation_bounds</t>
+    <t>height_end_start_relation_bounds</t>
   </si>
   <si>
     <t>f_regression_percentage_bounds</t>
@@ -100,25 +100,10 @@
     <t>[]</t>
   </si>
   <si>
-    <t>[-10, -0.2]</t>
-  </si>
-  <si>
-    <t>[0.2, 0.8]</t>
-  </si>
-  <si>
-    <t>[1.2, 10]</t>
+    <t>[0.1, 0.5]</t>
   </si>
   <si>
     <t>[0.9, 1.1]</t>
-  </si>
-  <si>
-    <t>[0.8, 1.2]</t>
-  </si>
-  <si>
-    <t>[0.8, 1.1]</t>
-  </si>
-  <si>
-    <t>[-20.0, 20.0]</t>
   </si>
   <si>
     <t>[-5.0, 5.0]</t>
@@ -585,19 +570,19 @@
         <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
         <v>41</v>
-      </c>
-      <c r="K2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -617,7 +602,7 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
@@ -626,13 +611,13 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
         <v>41</v>
-      </c>
-      <c r="K3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -652,7 +637,7 @@
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -661,13 +646,13 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
         <v>41</v>
-      </c>
-      <c r="K4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -687,22 +672,22 @@
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
         <v>41</v>
-      </c>
-      <c r="K5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -722,22 +707,22 @@
         <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" t="s">
         <v>41</v>
-      </c>
-      <c r="K6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -754,25 +739,25 @@
         <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -789,25 +774,25 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
         <v>36</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" t="s">
-        <v>41</v>
-      </c>
       <c r="K8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -824,25 +809,25 @@
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" t="s">
-        <v>37</v>
-      </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -862,7 +847,7 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G10" t="s">
         <v>25</v>
@@ -871,13 +856,13 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="K10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -897,7 +882,7 @@
         <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
@@ -906,13 +891,13 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -926,28 +911,28 @@
         <v>0.02</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="H12">
         <v>5</v>
       </c>
       <c r="I12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -961,28 +946,28 @@
         <v>0.02</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="H13">
         <v>5</v>
       </c>
       <c r="I13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J13" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
with cache and sound for upcoming breakouts...
</commit_message>
<xml_diff>
--- a/Gaming/Stocks/Pattern_Statistics/constraints.xlsx
+++ b/Gaming/Stocks/Pattern_Statistics/constraints.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
   <si>
     <t>Constraint</t>
   </si>
@@ -76,12 +76,6 @@
     <t>TKE down</t>
   </si>
   <si>
-    <t>Head-Shoulder</t>
-  </si>
-  <si>
-    <t>Inverse-Head-Shoulder</t>
-  </si>
-  <si>
     <t>[-50.0, -1.0]</t>
   </si>
   <si>
@@ -133,12 +127,6 @@
     <t>['OR', 'Upper_in &gt;= 3']</t>
   </si>
   <si>
-    <t>['AND', 'Low_in &gt;= 4', 'Upper_in &gt;= 1']</t>
-  </si>
-  <si>
-    <t>['AND', 'Upper_in &gt;= 4', 'Low_in &gt;= 1']</t>
-  </si>
-  <si>
     <t>['OR', ['Low_in', 'Upper_in', 'Low_in', 'Upper_in', 'Low_in'], ['Upper_in', 'Low_in', 'Upper_in', 'Low_in', 'Upper_in'], ['Low_in', 'Low_in', 'Upper_in', 'Upper_in', 'Low_in'], ['Upper_in', 'Upper_in', 'Low_in', 'Low_in', 'Upper_in']]</t>
   </si>
   <si>
@@ -149,12 +137,6 @@
   </si>
   <si>
     <t>['OR', ['Upper_on', 'Upper_in', 'Upper_on'], ['Upper_on', 'Upper_on', 'Upper_on']]</t>
-  </si>
-  <si>
-    <t>['OR', ['Low_on', 'Middle_in', 'Low_on', 'Upper_on', 'Low_on', 'Middle_in', 'Low_on'], ['Low_on', 'Middle_in', 'Low_in', 'Upper_on', 'Middle_in', 'Middle_in', 'Low_on']]</t>
-  </si>
-  <si>
-    <t>['OR', ['Upper_on', 'Middle_in', 'Upper_on', 'Low_on', 'Upper_on', 'Middle_in', 'Upper_on'], ['Upper_on', 'Middle_in', 'Upper_in', 'Low_on', 'Middle_in', 'Middle_in', 'Upper_on']]</t>
   </si>
 </sst>
 </file>
@@ -512,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -561,28 +543,28 @@
         <v>0.02</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -596,28 +578,28 @@
         <v>0.02</v>
       </c>
       <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -631,28 +613,28 @@
         <v>0.02</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -666,28 +648,28 @@
         <v>0.02</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -701,28 +683,28 @@
         <v>0.02</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -736,28 +718,28 @@
         <v>0.02</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -771,28 +753,28 @@
         <v>0.02</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>29</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
         <v>31</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>33</v>
-      </c>
       <c r="J8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -806,28 +788,28 @@
         <v>0.02</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
         <v>27</v>
       </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -841,28 +823,28 @@
         <v>0.02</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -876,98 +858,28 @@
         <v>0.02</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12">
-        <v>0.02</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12">
-        <v>5</v>
-      </c>
-      <c r="I12" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" t="s">
-        <v>39</v>
-      </c>
-      <c r="K12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
-        <v>0.02</v>
-      </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13">
-        <v>5</v>
-      </c>
-      <c r="I13" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" t="s">
         <v>40</v>
-      </c>
-      <c r="K13" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Constraints for triangle corrected
</commit_message>
<xml_diff>
--- a/Gaming/Stocks/Pattern_Statistics/constraints.xlsx
+++ b/Gaming/Stocks/Pattern_Statistics/constraints.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\OneDrive\GitHub\PycharmProjects\Gaming\Stocks\Pattern_Statistics\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_F6BE4EABDDC356CE8A160B464B62C01E4A4EBCBD" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{8507F4AA-077C-4B72-B714-437675BDAF4D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Constraints_2018-08-09" sheetId="1" r:id="rId1"/>
+    <sheet name="Constraints_2018-08-13" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="43">
   <si>
     <t>Constraint</t>
   </si>
@@ -82,22 +88,28 @@
     <t>[-1.0, 1.0]</t>
   </si>
   <si>
+    <t>[1.0, 50.0]</t>
+  </si>
+  <si>
+    <t>[-2.0, 2.0]</t>
+  </si>
+  <si>
+    <t>[2.0, 50.0]</t>
+  </si>
+  <si>
     <t>[-50.0, -2.0]</t>
   </si>
   <si>
-    <t>[2.0, 50.0]</t>
-  </si>
-  <si>
-    <t>[-2.0, 2.0]</t>
-  </si>
-  <si>
     <t>[]</t>
   </si>
   <si>
+    <t>[0.1, 0.8]</t>
+  </si>
+  <si>
+    <t>[0.9, 1.1]</t>
+  </si>
+  <si>
     <t>[0.1, 0.5]</t>
-  </si>
-  <si>
-    <t>[0.9, 1.1]</t>
   </si>
   <si>
     <t>[-5.0, 5.0]</t>
@@ -142,8 +154,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,12 +172,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -195,22 +213,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -252,7 +279,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -284,9 +311,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -318,6 +363,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -493,14 +556,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="198.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -546,28 +624,28 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -581,28 +659,28 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -613,31 +691,31 @@
         <v>0.02</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -648,31 +726,31 @@
         <v>0.02</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -683,31 +761,31 @@
         <v>0.02</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -718,31 +796,31 @@
         <v>0.02</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -753,31 +831,31 @@
         <v>0.02</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -788,31 +866,31 @@
         <v>0.02</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -823,31 +901,31 @@
         <v>0.02</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -858,28 +936,410 @@
         <v>0.02</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
         <v>25</v>
       </c>
-      <c r="F11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" t="s">
-        <v>22</v>
-      </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>0.02</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>0.02</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>0.02</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>0.02</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>0.02</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>0.02</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>0.02</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>0.02</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>0.02</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <v>0.02</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>